<commit_message>
New targets with aggregated MW data in IEA country groupings, all checks passing
</commit_message>
<xml_diff>
--- a/inst/extdata/Exemplar_Table.xlsx
+++ b/inst/extdata/Exemplar_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\PFUDatabase\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DBA685-6014-4569-866B-6758175E2A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9911E8BD-6648-4919-BC28-B2F11EE83758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24038" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24068" uniqueCount="524">
   <si>
     <t>Albania</t>
   </si>
@@ -2453,6 +2453,21 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2507,23 +2522,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3384,10 +3384,10 @@
   <dimension ref="A1:BL218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AJ20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="AI68" sqref="AI68:BL68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3400,197 +3400,197 @@
     <col min="62" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="64" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:64" s="44" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="43" t="s">
         <v>426</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="43" t="s">
         <v>443</v>
       </c>
-      <c r="D1" s="63">
+      <c r="D1" s="43">
         <v>1960</v>
       </c>
-      <c r="E1" s="63">
+      <c r="E1" s="43">
         <v>1961</v>
       </c>
-      <c r="F1" s="63">
+      <c r="F1" s="43">
         <v>1962</v>
       </c>
-      <c r="G1" s="63">
+      <c r="G1" s="43">
         <v>1963</v>
       </c>
-      <c r="H1" s="63">
+      <c r="H1" s="43">
         <v>1964</v>
       </c>
-      <c r="I1" s="63">
+      <c r="I1" s="43">
         <v>1965</v>
       </c>
-      <c r="J1" s="63">
+      <c r="J1" s="43">
         <v>1966</v>
       </c>
-      <c r="K1" s="63">
+      <c r="K1" s="43">
         <v>1967</v>
       </c>
-      <c r="L1" s="63">
+      <c r="L1" s="43">
         <v>1968</v>
       </c>
-      <c r="M1" s="63">
+      <c r="M1" s="43">
         <v>1969</v>
       </c>
-      <c r="N1" s="63">
+      <c r="N1" s="43">
         <v>1970</v>
       </c>
-      <c r="O1" s="63">
+      <c r="O1" s="43">
         <v>1971</v>
       </c>
-      <c r="P1" s="63">
+      <c r="P1" s="43">
         <v>1972</v>
       </c>
-      <c r="Q1" s="63">
+      <c r="Q1" s="43">
         <v>1973</v>
       </c>
-      <c r="R1" s="63">
+      <c r="R1" s="43">
         <v>1974</v>
       </c>
-      <c r="S1" s="63">
+      <c r="S1" s="43">
         <v>1975</v>
       </c>
-      <c r="T1" s="63">
+      <c r="T1" s="43">
         <v>1976</v>
       </c>
-      <c r="U1" s="63">
+      <c r="U1" s="43">
         <v>1977</v>
       </c>
-      <c r="V1" s="63">
+      <c r="V1" s="43">
         <v>1978</v>
       </c>
-      <c r="W1" s="63">
+      <c r="W1" s="43">
         <v>1979</v>
       </c>
-      <c r="X1" s="63">
+      <c r="X1" s="43">
         <v>1980</v>
       </c>
-      <c r="Y1" s="63">
+      <c r="Y1" s="43">
         <v>1981</v>
       </c>
-      <c r="Z1" s="63">
+      <c r="Z1" s="43">
         <v>1982</v>
       </c>
-      <c r="AA1" s="63">
+      <c r="AA1" s="43">
         <v>1983</v>
       </c>
-      <c r="AB1" s="63">
+      <c r="AB1" s="43">
         <v>1984</v>
       </c>
-      <c r="AC1" s="63">
+      <c r="AC1" s="43">
         <v>1985</v>
       </c>
-      <c r="AD1" s="63">
+      <c r="AD1" s="43">
         <v>1986</v>
       </c>
-      <c r="AE1" s="63">
+      <c r="AE1" s="43">
         <v>1987</v>
       </c>
-      <c r="AF1" s="63">
+      <c r="AF1" s="43">
         <v>1988</v>
       </c>
-      <c r="AG1" s="63">
+      <c r="AG1" s="43">
         <v>1989</v>
       </c>
-      <c r="AH1" s="63">
+      <c r="AH1" s="43">
         <v>1990</v>
       </c>
-      <c r="AI1" s="63">
+      <c r="AI1" s="43">
         <v>1991</v>
       </c>
-      <c r="AJ1" s="63">
+      <c r="AJ1" s="43">
         <v>1992</v>
       </c>
-      <c r="AK1" s="63">
+      <c r="AK1" s="43">
         <v>1993</v>
       </c>
-      <c r="AL1" s="63">
+      <c r="AL1" s="43">
         <v>1994</v>
       </c>
-      <c r="AM1" s="63">
+      <c r="AM1" s="43">
         <v>1995</v>
       </c>
-      <c r="AN1" s="63">
+      <c r="AN1" s="43">
         <v>1996</v>
       </c>
-      <c r="AO1" s="63">
+      <c r="AO1" s="43">
         <v>1997</v>
       </c>
-      <c r="AP1" s="63">
+      <c r="AP1" s="43">
         <v>1998</v>
       </c>
-      <c r="AQ1" s="63">
+      <c r="AQ1" s="43">
         <v>1999</v>
       </c>
-      <c r="AR1" s="63">
+      <c r="AR1" s="43">
         <v>2000</v>
       </c>
-      <c r="AS1" s="63">
+      <c r="AS1" s="43">
         <v>2001</v>
       </c>
-      <c r="AT1" s="63">
+      <c r="AT1" s="43">
         <v>2002</v>
       </c>
-      <c r="AU1" s="63">
+      <c r="AU1" s="43">
         <v>2003</v>
       </c>
-      <c r="AV1" s="63">
+      <c r="AV1" s="43">
         <v>2004</v>
       </c>
-      <c r="AW1" s="63">
+      <c r="AW1" s="43">
         <v>2005</v>
       </c>
-      <c r="AX1" s="63">
+      <c r="AX1" s="43">
         <v>2006</v>
       </c>
-      <c r="AY1" s="63">
+      <c r="AY1" s="43">
         <v>2007</v>
       </c>
-      <c r="AZ1" s="63">
+      <c r="AZ1" s="43">
         <v>2008</v>
       </c>
-      <c r="BA1" s="63">
+      <c r="BA1" s="43">
         <v>2009</v>
       </c>
-      <c r="BB1" s="63">
+      <c r="BB1" s="43">
         <v>2010</v>
       </c>
-      <c r="BC1" s="63">
+      <c r="BC1" s="43">
         <v>2011</v>
       </c>
-      <c r="BD1" s="63">
+      <c r="BD1" s="43">
         <v>2012</v>
       </c>
-      <c r="BE1" s="63">
+      <c r="BE1" s="43">
         <v>2013</v>
       </c>
-      <c r="BF1" s="63">
+      <c r="BF1" s="43">
         <v>2014</v>
       </c>
-      <c r="BG1" s="63">
+      <c r="BG1" s="43">
         <v>2015</v>
       </c>
-      <c r="BH1" s="63">
+      <c r="BH1" s="43">
         <v>2016</v>
       </c>
-      <c r="BI1" s="63">
+      <c r="BI1" s="43">
         <v>2017</v>
       </c>
-      <c r="BJ1" s="63">
+      <c r="BJ1" s="43">
         <v>2018</v>
       </c>
-      <c r="BK1" s="63">
+      <c r="BK1" s="43">
         <v>2019</v>
       </c>
-      <c r="BL1" s="63">
+      <c r="BL1" s="43">
         <v>2020</v>
       </c>
     </row>
@@ -16501,6 +16501,96 @@
       <c r="AH68" s="20" t="s">
         <v>57</v>
       </c>
+      <c r="AI68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BD68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BK68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BL68" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="69" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -18831,196 +18921,196 @@
       </c>
     </row>
     <row r="81" spans="1:64" x14ac:dyDescent="0.2">
-      <c r="A81" s="65" t="s">
+      <c r="A81" s="45" t="s">
         <v>452</v>
       </c>
-      <c r="B81" s="65" t="s">
+      <c r="B81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C81" s="65" t="s">
+      <c r="C81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="D81" s="65" t="s">
+      <c r="D81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="E81" s="65" t="s">
+      <c r="E81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="F81" s="65" t="s">
+      <c r="F81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="G81" s="65" t="s">
+      <c r="G81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="H81" s="65" t="s">
+      <c r="H81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="I81" s="65" t="s">
+      <c r="I81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="J81" s="65" t="s">
+      <c r="J81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="K81" s="65" t="s">
+      <c r="K81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="L81" s="65" t="s">
+      <c r="L81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="M81" s="65" t="s">
+      <c r="M81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="N81" s="65" t="s">
+      <c r="N81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="O81" s="65" t="s">
+      <c r="O81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="P81" s="65" t="s">
+      <c r="P81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="Q81" s="65" t="s">
+      <c r="Q81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="R81" s="65" t="s">
+      <c r="R81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="S81" s="65" t="s">
+      <c r="S81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="T81" s="65" t="s">
+      <c r="T81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="U81" s="65" t="s">
+      <c r="U81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="V81" s="65" t="s">
+      <c r="V81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="W81" s="65" t="s">
+      <c r="W81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="X81" s="65" t="s">
+      <c r="X81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="Y81" s="65" t="s">
+      <c r="Y81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="Z81" s="65" t="s">
+      <c r="Z81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AA81" s="65" t="s">
+      <c r="AA81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AB81" s="65" t="s">
+      <c r="AB81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AC81" s="65" t="s">
+      <c r="AC81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AD81" s="65" t="s">
+      <c r="AD81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AE81" s="65" t="s">
+      <c r="AE81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AF81" s="65" t="s">
+      <c r="AF81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AG81" s="65" t="s">
+      <c r="AG81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AH81" s="65" t="s">
+      <c r="AH81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AI81" s="65" t="s">
+      <c r="AI81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AJ81" s="65" t="s">
+      <c r="AJ81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AK81" s="65" t="s">
+      <c r="AK81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AL81" s="65" t="s">
+      <c r="AL81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AM81" s="65" t="s">
+      <c r="AM81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AN81" s="65" t="s">
+      <c r="AN81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AO81" s="65" t="s">
+      <c r="AO81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AP81" s="65" t="s">
+      <c r="AP81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AQ81" s="65" t="s">
+      <c r="AQ81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AR81" s="65" t="s">
+      <c r="AR81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AS81" s="65" t="s">
+      <c r="AS81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AT81" s="65" t="s">
+      <c r="AT81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AU81" s="65" t="s">
+      <c r="AU81" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="AV81" s="65" t="s">
+      <c r="AV81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="AW81" s="65" t="s">
+      <c r="AW81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="AX81" s="65" t="s">
+      <c r="AX81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="AY81" s="65" t="s">
+      <c r="AY81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="AZ81" s="65" t="s">
+      <c r="AZ81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BA81" s="65" t="s">
+      <c r="BA81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BB81" s="65" t="s">
+      <c r="BB81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BC81" s="65" t="s">
+      <c r="BC81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BD81" s="65" t="s">
+      <c r="BD81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BE81" s="65" t="s">
+      <c r="BE81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BF81" s="65" t="s">
+      <c r="BF81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BG81" s="65" t="s">
+      <c r="BG81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BH81" s="65" t="s">
+      <c r="BH81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BI81" s="65" t="s">
+      <c r="BI81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BJ81" s="65" t="s">
+      <c r="BJ81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BK81" s="65" t="s">
+      <c r="BK81" s="45" t="s">
         <v>332</v>
       </c>
-      <c r="BL81" s="65" t="s">
+      <c r="BL81" s="45" t="s">
         <v>332</v>
       </c>
     </row>
@@ -19606,7 +19696,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="85" spans="1:64" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:64" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>447</v>
       </c>
@@ -33381,196 +33471,196 @@
       </c>
     </row>
     <row r="156" spans="1:64" x14ac:dyDescent="0.2">
-      <c r="A156" s="65" t="s">
+      <c r="A156" s="45" t="s">
         <v>455</v>
       </c>
-      <c r="B156" s="65" t="s">
+      <c r="B156" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="C156" s="65" t="s">
+      <c r="C156" s="45" t="s">
         <v>503</v>
       </c>
-      <c r="D156" s="65" t="s">
+      <c r="D156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="E156" s="65" t="s">
+      <c r="E156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="F156" s="65" t="s">
+      <c r="F156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="G156" s="65" t="s">
+      <c r="G156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="H156" s="65" t="s">
+      <c r="H156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="I156" s="65" t="s">
+      <c r="I156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="J156" s="65" t="s">
+      <c r="J156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="K156" s="65" t="s">
+      <c r="K156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="L156" s="65" t="s">
+      <c r="L156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="M156" s="65" t="s">
+      <c r="M156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="N156" s="65" t="s">
+      <c r="N156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="O156" s="65" t="s">
+      <c r="O156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="P156" s="65" t="s">
+      <c r="P156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="Q156" s="65" t="s">
+      <c r="Q156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="R156" s="65" t="s">
+      <c r="R156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="S156" s="65" t="s">
+      <c r="S156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="T156" s="65" t="s">
+      <c r="T156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="U156" s="65" t="s">
+      <c r="U156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="V156" s="65" t="s">
+      <c r="V156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="W156" s="65" t="s">
+      <c r="W156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="X156" s="65" t="s">
+      <c r="X156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="Y156" s="65" t="s">
+      <c r="Y156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="Z156" s="65" t="s">
+      <c r="Z156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AA156" s="65" t="s">
+      <c r="AA156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AB156" s="65" t="s">
+      <c r="AB156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AC156" s="65" t="s">
+      <c r="AC156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AD156" s="65" t="s">
+      <c r="AD156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AE156" s="65" t="s">
+      <c r="AE156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AF156" s="65" t="s">
+      <c r="AF156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AG156" s="65" t="s">
+      <c r="AG156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AH156" s="65" t="s">
+      <c r="AH156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AI156" s="65" t="s">
+      <c r="AI156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AJ156" s="65" t="s">
+      <c r="AJ156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AK156" s="65" t="s">
+      <c r="AK156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AL156" s="65" t="s">
+      <c r="AL156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AM156" s="65" t="s">
+      <c r="AM156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AN156" s="65" t="s">
+      <c r="AN156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AO156" s="65" t="s">
+      <c r="AO156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AP156" s="65" t="s">
+      <c r="AP156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AQ156" s="65" t="s">
+      <c r="AQ156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AR156" s="65" t="s">
+      <c r="AR156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AS156" s="65" t="s">
+      <c r="AS156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AT156" s="65" t="s">
+      <c r="AT156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AU156" s="65" t="s">
+      <c r="AU156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AV156" s="65" t="s">
+      <c r="AV156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AW156" s="65" t="s">
+      <c r="AW156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AX156" s="65" t="s">
+      <c r="AX156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AY156" s="65" t="s">
+      <c r="AY156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="AZ156" s="65" t="s">
+      <c r="AZ156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BA156" s="65" t="s">
+      <c r="BA156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BB156" s="65" t="s">
+      <c r="BB156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BC156" s="65" t="s">
+      <c r="BC156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BD156" s="65" t="s">
+      <c r="BD156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BE156" s="65" t="s">
+      <c r="BE156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BF156" s="65" t="s">
+      <c r="BF156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BG156" s="65" t="s">
+      <c r="BG156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BH156" s="65" t="s">
+      <c r="BH156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BI156" s="65" t="s">
+      <c r="BI156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BJ156" s="65" t="s">
+      <c r="BJ156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BK156" s="65" t="s">
+      <c r="BK156" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="BL156" s="65" t="s">
+      <c r="BL156" s="45" t="s">
         <v>234</v>
       </c>
     </row>
@@ -34156,7 +34246,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="160" spans="1:64" s="65" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:64" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>454</v>
       </c>
@@ -77336,18 +77426,18 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44"/>
-      <c r="H3" s="51" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
+      <c r="H3" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="58"/>
       <c r="N3" s="2" t="s">
         <v>251</v>
       </c>
@@ -77359,14 +77449,14 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="56"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="61"/>
       <c r="N4" s="2" t="s">
         <v>253</v>
       </c>
@@ -77378,14 +77468,14 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="59"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="64"/>
       <c r="N5" s="2" t="s">
         <v>254</v>
       </c>
@@ -77427,38 +77517,38 @@
     </row>
     <row r="8" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="44"/>
-      <c r="H9" s="51" t="s">
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
+      <c r="H9" s="56" t="s">
         <v>343</v>
       </c>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="53"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
     </row>
     <row r="10" spans="2:16" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="45"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="47"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="61"/>
     </row>
     <row r="11" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="50"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="55"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="19"/>
@@ -77467,63 +77557,63 @@
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="2:16" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="65" t="s">
         <v>349</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
       <c r="H13" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="H15" s="51" t="s">
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="H15" s="56" t="s">
         <v>347</v>
       </c>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="53"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="58"/>
     </row>
     <row r="16" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="54"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="56"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="61"/>
     </row>
     <row r="17" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="44"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="59"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="49"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="64"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
     </row>
     <row r="19" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="48"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="50"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
       <c r="H19" t="s">
         <v>345</v>
       </c>
@@ -77533,109 +77623,114 @@
       <c r="B21" t="s">
         <v>351</v>
       </c>
-      <c r="H21" s="51" t="s">
+      <c r="H21" s="56" t="s">
         <v>346</v>
       </c>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="53"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="58"/>
     </row>
     <row r="22" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H22" s="54"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="56"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="61"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="44"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="59"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="49"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="64"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="45"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="47"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="48"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="50"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="55"/>
       <c r="H25" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
     </row>
     <row r="34" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="44"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="49"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="47"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="52"/>
     </row>
     <row r="37" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="48"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="50"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B9:E11"/>
+    <mergeCell ref="H3:K5"/>
+    <mergeCell ref="H9:K11"/>
+    <mergeCell ref="B27:E29"/>
     <mergeCell ref="B31:E33"/>
     <mergeCell ref="B35:E37"/>
     <mergeCell ref="H15:K17"/>
@@ -77643,11 +77738,6 @@
     <mergeCell ref="B13:E15"/>
     <mergeCell ref="B17:E19"/>
     <mergeCell ref="B23:E25"/>
-    <mergeCell ref="B3:E5"/>
-    <mergeCell ref="B9:E11"/>
-    <mergeCell ref="H3:K5"/>
-    <mergeCell ref="H9:K11"/>
-    <mergeCell ref="B27:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -78181,6 +78271,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060B7F65646EC444FB25DA4F5E743F4A7" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f076e5527b1f1957b74e8a9e048be81">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="77d41baf-5ecc-4842-ba36-0ed33caf7049" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="626007ce907977db909c72728f6668c7" ns3:_="">
     <xsd:import namespace="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
@@ -78326,22 +78431,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83F7A5DA-1B98-4A64-9D1E-26B3B73D80C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828852AD-0200-491F-83D2-C0A0FDC8BB33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA1D15D9-8398-4015-A6D6-79D5997F5C5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -78357,28 +78471,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828852AD-0200-491F-83D2-C0A0FDC8BB33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83F7A5DA-1B98-4A64-9D1E-26B3B73D80C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="77d41baf-5ecc-4842-ba36-0ed33caf7049"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>